<commit_message>
removed key and value from excel
</commit_message>
<xml_diff>
--- a/build/libs/ForHashMap.xlsx
+++ b/build/libs/ForHashMap.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="67">
   <si>
     <t>cloud computing</t>
   </si>
@@ -202,12 +202,6 @@
   </si>
   <si>
     <t>psycholog</t>
-  </si>
-  <si>
-    <t>Key</t>
-  </si>
-  <si>
-    <t>Value</t>
   </si>
   <si>
     <t>cloud_computing</t>
@@ -561,22 +555,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B57"/>
+  <dimension ref="A2:B57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B1" t="s">
-        <v>63</v>
-      </c>
-    </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>35</v>
@@ -606,7 +592,7 @@
         <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -614,7 +600,7 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -638,7 +624,7 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -646,7 +632,7 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -702,7 +688,7 @@
         <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -710,7 +696,7 @@
         <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -718,7 +704,7 @@
         <v>53</v>
       </c>
       <c r="B19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -726,7 +712,7 @@
         <v>54</v>
       </c>
       <c r="B20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -734,7 +720,7 @@
         <v>59</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -822,7 +808,7 @@
         <v>19</v>
       </c>
       <c r="B32" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -830,7 +816,7 @@
         <v>20</v>
       </c>
       <c r="B33" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -838,7 +824,7 @@
         <v>21</v>
       </c>
       <c r="B34" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -846,7 +832,7 @@
         <v>22</v>
       </c>
       <c r="B35" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -854,7 +840,7 @@
         <v>23</v>
       </c>
       <c r="B36" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -862,7 +848,7 @@
         <v>24</v>
       </c>
       <c r="B37" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -870,7 +856,7 @@
         <v>25</v>
       </c>
       <c r="B38" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -1006,7 +992,7 @@
         <v>45</v>
       </c>
       <c r="B55" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
@@ -1014,7 +1000,7 @@
         <v>46</v>
       </c>
       <c r="B56" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
@@ -1022,7 +1008,7 @@
         <v>47</v>
       </c>
       <c r="B57" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>